<commit_message>
finalizando o doc de especificao de casos de uso de teste, por enquanto
</commit_message>
<xml_diff>
--- a/outros/Especificação Caso de Uso Testes/Esp. Casos de Uso de Testes.xlsx
+++ b/outros/Especificação Caso de Uso Testes/Esp. Casos de Uso de Testes.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Usuario\Desktop\e-commerce-Livros\outros\Especificação Caso de Uso Testes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{063F61E4-8E0F-403A-BF83-FFA3658A1BCB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9011F195-753C-454C-A7E3-23B2160B6071}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="297" uniqueCount="124">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="334" uniqueCount="152">
   <si>
     <t>Checklist Plano de Testes</t>
   </si>
@@ -50,9 +50,6 @@
   </si>
   <si>
     <t>Resposta**</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Observações </t>
   </si>
   <si>
     <t>Severidade (*)</t>
@@ -353,9 +350,6 @@
     <t xml:space="preserve">Inserir um valor, para pagar, menor que o valor total da compra </t>
   </si>
   <si>
-    <t>O sistema não deve deixar o usuário fazer isso</t>
-  </si>
-  <si>
     <t>Inserir quantidade monetária correta para o pagamento dos itens do Carrinho, R$ 139,70</t>
   </si>
   <si>
@@ -392,13 +386,7 @@
     <t>Voltar para a página da Conta do Cliente</t>
   </si>
   <si>
-    <t>É esperado que dê erro nesse passo</t>
-  </si>
-  <si>
     <t>Apertar o Botão "Meus cupons"</t>
-  </si>
-  <si>
-    <t>Deve exibir os cupons gerados a partir da aprovação da Troca que o Cliente Solicitou</t>
   </si>
   <si>
     <t>Pesquisar o livro "1984" na barra de pesquisa</t>
@@ -440,16 +428,10 @@
     <t>Adicionar mais um cupom de 30 reais</t>
   </si>
   <si>
-    <t>O valor da compra já está zerado, então o sistema não deve permitir o uso de mais cupons</t>
-  </si>
-  <si>
     <t>Finalizar a compra</t>
   </si>
   <si>
     <t>Repetir o passo 12 e 28</t>
-  </si>
-  <si>
-    <t>Um cupom de 50 reais não deve mais estar disponível, e um cupom de 25 reais deve aparecer devido ao valor excedente da compra que foi realizada anteriormente</t>
   </si>
   <si>
     <t>Apertar o botão "Meus Pedidos" e ver o Pedido mais recente</t>
@@ -468,6 +450,108 @@
   </si>
   <si>
     <t>Baixa</t>
+  </si>
+  <si>
+    <t>Resultado Esperado</t>
+  </si>
+  <si>
+    <t>Observações</t>
+  </si>
+  <si>
+    <t>A página do produto carregada e funcional</t>
+  </si>
+  <si>
+    <t>O Carrinho com os itens adicionados</t>
+  </si>
+  <si>
+    <t>Alteração da quantidade dos produtos do carrinho</t>
+  </si>
+  <si>
+    <t>A Exclusão de um item do Carrinho</t>
+  </si>
+  <si>
+    <t>A página de busca retornando livros com base no nome pesquisado</t>
+  </si>
+  <si>
+    <t>Diferentes itens adicionados ao Carrinho</t>
+  </si>
+  <si>
+    <t>A página de compra carregada e funcionando</t>
+  </si>
+  <si>
+    <t>Endereço de entrega do cliente selecionado</t>
+  </si>
+  <si>
+    <t>O sistema deve exibir um alerta de erro, avisando que isso não é permitido</t>
+  </si>
+  <si>
+    <t>Foi implementado essa lógica na Service dos Pedidos</t>
+  </si>
+  <si>
+    <t>O sistema deve exibir um alerta de erro, não deixando o usuário prosseguir</t>
+  </si>
+  <si>
+    <t>Pedido realizado com sucesso</t>
+  </si>
+  <si>
+    <t>Modal aparece na tela do cliente informando o código do pedido e redirecionando o mesmo para a página da Conta</t>
+  </si>
+  <si>
+    <t>Implementada a resposta da API para exibir o código do Pedido</t>
+  </si>
+  <si>
+    <t>Página dos pedidos do cliente carregada</t>
+  </si>
+  <si>
+    <t>Pedido em questão aparecendo na tela</t>
+  </si>
+  <si>
+    <t>Exbição do Modal de confirmação e posteriormente a alteração do status</t>
+  </si>
+  <si>
+    <t>Tela do Administrador Carregada</t>
+  </si>
+  <si>
+    <t>Pedido do cliente em questão carregada com sucesso</t>
+  </si>
+  <si>
+    <t>Exibição do modal de confimação e a alteração do Status</t>
+  </si>
+  <si>
+    <t>Página do Cliente Carregada</t>
+  </si>
+  <si>
+    <t>Exibição do modal de confimação, este dando a possibilidade de retornar os itens trocados ao estoque ou não, e a alteração do Status</t>
+  </si>
+  <si>
+    <t>Página dos cupons do cliente Carregado</t>
+  </si>
+  <si>
+    <t>Página de amostragem do cupom implementada</t>
+  </si>
+  <si>
+    <t>A página do produto carregada e funcional, e exibindo o valor de 75 reais</t>
+  </si>
+  <si>
+    <t>Página de pagamento apenas daquele livro específico carregada</t>
+  </si>
+  <si>
+    <t>Cupom adicionado com sucesso, mostrando o desconto devido da área do extrato</t>
+  </si>
+  <si>
+    <t>Modal de erro deve aparecer informando que não é possível adicionar mais cupons</t>
+  </si>
+  <si>
+    <t>Modal de Pedido Realizado com sucesso, mostrando o código do pedido e redirecionando o usuário pra Página da Conta</t>
+  </si>
+  <si>
+    <t>Página dos pedidos do cliente carregada mostrando seus pedidos</t>
+  </si>
+  <si>
+    <t>Modal do pedido aberto, informando a forma de pagamento como: "Cupom"</t>
+  </si>
+  <si>
+    <t>Lógica da forma de pagamento implementada</t>
   </si>
 </sst>
 </file>
@@ -1233,7 +1317,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="123">
+  <cellXfs count="122">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1361,18 +1445,13 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="1" fontId="7" fillId="3" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="3" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="3" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="7" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -1384,10 +1463,6 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="7" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="7" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="8" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -1401,7 +1476,6 @@
     <xf numFmtId="0" fontId="19" fillId="3" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="9" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="9" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="9" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -1441,28 +1515,11 @@
     <xf numFmtId="0" fontId="4" fillId="9" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="14" fontId="20" fillId="5" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="6" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="20" fillId="5" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="6" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="18" fillId="10" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="21" fillId="3" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -1479,13 +1536,45 @@
     <xf numFmtId="164" fontId="10" fillId="3" borderId="29" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="22" fillId="5" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="23" fillId="6" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="23" fillId="6" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="20" fillId="5" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="6" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="14" fillId="6" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="20" fillId="5" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="8" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1787,8 +1876,8 @@
   </sheetPr>
   <dimension ref="A1:Z1037"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" view="pageLayout" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D54" sqref="D54"/>
+    <sheetView showGridLines="0" tabSelected="1" view="pageLayout" topLeftCell="A16" zoomScale="90" zoomScaleNormal="100" zoomScalePageLayoutView="90" workbookViewId="0">
+      <selection activeCell="A65" sqref="A65"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" outlineLevelRow="1" x14ac:dyDescent="0.2"/>
@@ -1799,7 +1888,7 @@
     <col min="4" max="4" width="53" customWidth="1"/>
     <col min="5" max="8" width="9.7109375" customWidth="1"/>
     <col min="9" max="9" width="37.85546875" customWidth="1"/>
-    <col min="10" max="10" width="9.140625" customWidth="1"/>
+    <col min="10" max="10" width="30.140625" customWidth="1"/>
     <col min="11" max="26" width="8" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1862,16 +1951,16 @@
       <c r="Z2" s="3"/>
     </row>
     <row r="3" spans="1:26" ht="3" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="82"/>
-      <c r="B3" s="83"/>
-      <c r="C3" s="83"/>
-      <c r="D3" s="83"/>
-      <c r="E3" s="83"/>
-      <c r="F3" s="83"/>
-      <c r="G3" s="83"/>
-      <c r="H3" s="83"/>
-      <c r="I3" s="83"/>
-      <c r="J3" s="84"/>
+      <c r="A3" s="74"/>
+      <c r="B3" s="75"/>
+      <c r="C3" s="75"/>
+      <c r="D3" s="75"/>
+      <c r="E3" s="75"/>
+      <c r="F3" s="75"/>
+      <c r="G3" s="75"/>
+      <c r="H3" s="75"/>
+      <c r="I3" s="75"/>
+      <c r="J3" s="76"/>
       <c r="K3" s="3"/>
       <c r="L3" s="3"/>
       <c r="M3" s="3"/>
@@ -1890,20 +1979,20 @@
       <c r="Z3" s="3"/>
     </row>
     <row r="4" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="85"/>
-      <c r="B4" s="86"/>
-      <c r="C4" s="86"/>
-      <c r="D4" s="87" t="s">
+      <c r="A4" s="77"/>
+      <c r="B4" s="78"/>
+      <c r="C4" s="78"/>
+      <c r="D4" s="79" t="s">
         <v>1</v>
       </c>
-      <c r="E4" s="108" t="s">
-        <v>74</v>
-      </c>
-      <c r="F4" s="109"/>
-      <c r="G4" s="109"/>
-      <c r="H4" s="109"/>
-      <c r="I4" s="107"/>
-      <c r="J4" s="88"/>
+      <c r="E4" s="109" t="s">
+        <v>73</v>
+      </c>
+      <c r="F4" s="110"/>
+      <c r="G4" s="110"/>
+      <c r="H4" s="110"/>
+      <c r="I4" s="111"/>
+      <c r="J4" s="80"/>
       <c r="K4" s="3"/>
       <c r="L4" s="3"/>
       <c r="M4" s="3"/>
@@ -1922,16 +2011,16 @@
       <c r="Z4" s="3"/>
     </row>
     <row r="5" spans="1:26" ht="3" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="85"/>
-      <c r="B5" s="86"/>
-      <c r="C5" s="86"/>
-      <c r="D5" s="89"/>
-      <c r="E5" s="90"/>
-      <c r="F5" s="90"/>
-      <c r="G5" s="90"/>
-      <c r="H5" s="90"/>
-      <c r="I5" s="90"/>
-      <c r="J5" s="88"/>
+      <c r="A5" s="77"/>
+      <c r="B5" s="78"/>
+      <c r="C5" s="78"/>
+      <c r="D5" s="81"/>
+      <c r="E5" s="82"/>
+      <c r="F5" s="82"/>
+      <c r="G5" s="82"/>
+      <c r="H5" s="82"/>
+      <c r="I5" s="82"/>
+      <c r="J5" s="80"/>
       <c r="K5" s="3"/>
       <c r="L5" s="3"/>
       <c r="M5" s="3"/>
@@ -1950,20 +2039,20 @@
       <c r="Z5" s="3"/>
     </row>
     <row r="6" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="85"/>
-      <c r="B6" s="86"/>
-      <c r="C6" s="86"/>
-      <c r="D6" s="87" t="s">
+      <c r="A6" s="77"/>
+      <c r="B6" s="78"/>
+      <c r="C6" s="78"/>
+      <c r="D6" s="79" t="s">
         <v>2</v>
       </c>
-      <c r="E6" s="108" t="s">
-        <v>75</v>
-      </c>
-      <c r="F6" s="109"/>
-      <c r="G6" s="109"/>
-      <c r="H6" s="109"/>
-      <c r="I6" s="107"/>
-      <c r="J6" s="88"/>
+      <c r="E6" s="109" t="s">
+        <v>74</v>
+      </c>
+      <c r="F6" s="110"/>
+      <c r="G6" s="110"/>
+      <c r="H6" s="110"/>
+      <c r="I6" s="111"/>
+      <c r="J6" s="80"/>
       <c r="K6" s="3"/>
       <c r="L6" s="3"/>
       <c r="M6" s="3"/>
@@ -1982,16 +2071,16 @@
       <c r="Z6" s="3"/>
     </row>
     <row r="7" spans="1:26" ht="3" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="85"/>
-      <c r="B7" s="86"/>
-      <c r="C7" s="86"/>
-      <c r="D7" s="87"/>
-      <c r="E7" s="90"/>
-      <c r="F7" s="90"/>
-      <c r="G7" s="90"/>
-      <c r="H7" s="90"/>
-      <c r="I7" s="90"/>
-      <c r="J7" s="88"/>
+      <c r="A7" s="77"/>
+      <c r="B7" s="78"/>
+      <c r="C7" s="78"/>
+      <c r="D7" s="79"/>
+      <c r="E7" s="82"/>
+      <c r="F7" s="82"/>
+      <c r="G7" s="82"/>
+      <c r="H7" s="82"/>
+      <c r="I7" s="82"/>
+      <c r="J7" s="80"/>
       <c r="K7" s="3"/>
       <c r="L7" s="3"/>
       <c r="M7" s="3"/>
@@ -2010,20 +2099,20 @@
       <c r="Z7" s="3"/>
     </row>
     <row r="8" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="85"/>
-      <c r="B8" s="86"/>
-      <c r="C8" s="86"/>
-      <c r="D8" s="87" t="s">
+      <c r="A8" s="77"/>
+      <c r="B8" s="78"/>
+      <c r="C8" s="78"/>
+      <c r="D8" s="79" t="s">
         <v>3</v>
       </c>
-      <c r="E8" s="106">
+      <c r="E8" s="112">
         <v>45798</v>
       </c>
-      <c r="F8" s="107"/>
-      <c r="G8" s="90"/>
-      <c r="H8" s="90"/>
-      <c r="I8" s="90"/>
-      <c r="J8" s="88"/>
+      <c r="F8" s="111"/>
+      <c r="G8" s="82"/>
+      <c r="H8" s="82"/>
+      <c r="I8" s="82"/>
+      <c r="J8" s="80"/>
       <c r="K8" s="3"/>
       <c r="L8" s="3"/>
       <c r="M8" s="3"/>
@@ -2042,16 +2131,16 @@
       <c r="Z8" s="3"/>
     </row>
     <row r="9" spans="1:26" ht="3" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="85"/>
-      <c r="B9" s="86"/>
-      <c r="C9" s="86"/>
-      <c r="D9" s="87"/>
-      <c r="E9" s="90"/>
-      <c r="F9" s="90"/>
-      <c r="G9" s="90"/>
-      <c r="H9" s="90"/>
-      <c r="I9" s="90"/>
-      <c r="J9" s="88"/>
+      <c r="A9" s="77"/>
+      <c r="B9" s="78"/>
+      <c r="C9" s="78"/>
+      <c r="D9" s="79"/>
+      <c r="E9" s="82"/>
+      <c r="F9" s="82"/>
+      <c r="G9" s="82"/>
+      <c r="H9" s="82"/>
+      <c r="I9" s="82"/>
+      <c r="J9" s="80"/>
       <c r="K9" s="3"/>
       <c r="L9" s="3"/>
       <c r="M9" s="3"/>
@@ -2070,18 +2159,18 @@
       <c r="Z9" s="3"/>
     </row>
     <row r="10" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="85"/>
-      <c r="B10" s="86"/>
-      <c r="C10" s="86"/>
-      <c r="D10" s="87" t="s">
+      <c r="A10" s="77"/>
+      <c r="B10" s="78"/>
+      <c r="C10" s="78"/>
+      <c r="D10" s="79" t="s">
         <v>4</v>
       </c>
-      <c r="E10" s="105"/>
-      <c r="F10" s="67"/>
-      <c r="G10" s="67"/>
-      <c r="H10" s="67"/>
-      <c r="I10" s="68"/>
-      <c r="J10" s="88"/>
+      <c r="E10" s="113"/>
+      <c r="F10" s="114"/>
+      <c r="G10" s="114"/>
+      <c r="H10" s="114"/>
+      <c r="I10" s="115"/>
+      <c r="J10" s="80"/>
       <c r="K10" s="3"/>
       <c r="L10" s="3"/>
       <c r="M10" s="3"/>
@@ -2100,16 +2189,16 @@
       <c r="Z10" s="3"/>
     </row>
     <row r="11" spans="1:26" ht="3" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="85"/>
-      <c r="B11" s="86"/>
-      <c r="C11" s="86"/>
-      <c r="D11" s="89"/>
-      <c r="E11" s="90"/>
-      <c r="F11" s="90"/>
-      <c r="G11" s="90"/>
-      <c r="H11" s="90"/>
-      <c r="I11" s="90"/>
-      <c r="J11" s="88"/>
+      <c r="A11" s="77"/>
+      <c r="B11" s="78"/>
+      <c r="C11" s="78"/>
+      <c r="D11" s="81"/>
+      <c r="E11" s="82"/>
+      <c r="F11" s="82"/>
+      <c r="G11" s="82"/>
+      <c r="H11" s="82"/>
+      <c r="I11" s="82"/>
+      <c r="J11" s="80"/>
       <c r="K11" s="3"/>
       <c r="L11" s="3"/>
       <c r="M11" s="3"/>
@@ -2128,16 +2217,16 @@
       <c r="Z11" s="3"/>
     </row>
     <row r="12" spans="1:26" ht="3" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="91"/>
-      <c r="B12" s="92"/>
-      <c r="C12" s="92"/>
-      <c r="D12" s="92"/>
-      <c r="E12" s="92"/>
-      <c r="F12" s="92"/>
-      <c r="G12" s="92"/>
-      <c r="H12" s="92"/>
-      <c r="I12" s="92"/>
-      <c r="J12" s="93"/>
+      <c r="A12" s="83"/>
+      <c r="B12" s="84"/>
+      <c r="C12" s="84"/>
+      <c r="D12" s="84"/>
+      <c r="E12" s="84"/>
+      <c r="F12" s="84"/>
+      <c r="G12" s="84"/>
+      <c r="H12" s="84"/>
+      <c r="I12" s="84"/>
+      <c r="J12" s="85"/>
       <c r="K12" s="3"/>
       <c r="L12" s="3"/>
       <c r="M12" s="3"/>
@@ -2212,20 +2301,22 @@
       <c r="Z14" s="3"/>
     </row>
     <row r="15" spans="1:26" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="69"/>
-      <c r="B15" s="72"/>
-      <c r="C15" s="73"/>
-      <c r="D15" s="73"/>
-      <c r="E15" s="74" t="s">
+      <c r="A15" s="64"/>
+      <c r="B15" s="67"/>
+      <c r="C15" s="68"/>
+      <c r="D15" s="68"/>
+      <c r="E15" s="116" t="s">
         <v>5</v>
       </c>
-      <c r="F15" s="75"/>
-      <c r="G15" s="75"/>
-      <c r="H15" s="75"/>
-      <c r="I15" s="74" t="s">
-        <v>6</v>
-      </c>
-      <c r="J15" s="75"/>
+      <c r="F15" s="117"/>
+      <c r="G15" s="117"/>
+      <c r="H15" s="117"/>
+      <c r="I15" s="118" t="s">
+        <v>118</v>
+      </c>
+      <c r="J15" s="120" t="s">
+        <v>119</v>
+      </c>
       <c r="K15" s="3"/>
       <c r="L15" s="3"/>
       <c r="M15" s="3"/>
@@ -2244,28 +2335,28 @@
       <c r="Z15" s="3"/>
     </row>
     <row r="16" spans="1:26" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="70" t="s">
+      <c r="A16" s="65" t="s">
+        <v>6</v>
+      </c>
+      <c r="B16" s="69" t="s">
         <v>7</v>
       </c>
-      <c r="B16" s="76" t="s">
+      <c r="C16" s="70"/>
+      <c r="D16" s="71"/>
+      <c r="E16" s="72" t="s">
         <v>8</v>
       </c>
-      <c r="C16" s="77"/>
-      <c r="D16" s="78"/>
-      <c r="E16" s="79" t="s">
+      <c r="F16" s="72" t="s">
         <v>9</v>
       </c>
-      <c r="F16" s="79" t="s">
+      <c r="G16" s="72" t="s">
         <v>10</v>
       </c>
-      <c r="G16" s="79" t="s">
+      <c r="H16" s="72" t="s">
         <v>11</v>
       </c>
-      <c r="H16" s="79" t="s">
-        <v>12</v>
-      </c>
-      <c r="I16" s="75"/>
-      <c r="J16" s="75"/>
+      <c r="I16" s="119"/>
+      <c r="J16" s="121"/>
       <c r="K16" s="3"/>
       <c r="L16" s="3"/>
       <c r="M16" s="3"/>
@@ -2284,20 +2375,20 @@
       <c r="Z16" s="3"/>
     </row>
     <row r="17" spans="1:26" ht="11.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="71"/>
-      <c r="B17" s="94">
+      <c r="A17" s="66"/>
+      <c r="B17" s="86">
         <v>1</v>
       </c>
-      <c r="C17" s="95" t="s">
-        <v>13</v>
-      </c>
-      <c r="D17" s="96"/>
-      <c r="E17" s="97"/>
-      <c r="F17" s="97"/>
-      <c r="G17" s="97"/>
-      <c r="H17" s="97"/>
-      <c r="I17" s="96"/>
-      <c r="J17" s="98"/>
+      <c r="C17" s="87" t="s">
+        <v>12</v>
+      </c>
+      <c r="D17" s="88"/>
+      <c r="E17" s="89"/>
+      <c r="F17" s="89"/>
+      <c r="G17" s="89"/>
+      <c r="H17" s="89"/>
+      <c r="I17" s="88"/>
+      <c r="J17" s="90"/>
       <c r="K17" s="4"/>
       <c r="L17" s="4"/>
       <c r="M17" s="4"/>
@@ -2315,25 +2406,27 @@
       <c r="Y17" s="4"/>
       <c r="Z17" s="4"/>
     </row>
-    <row r="18" spans="1:26" ht="23.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="122" t="s">
-        <v>121</v>
+    <row r="18" spans="1:26" ht="27.75" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.2">
+      <c r="A18" s="104" t="s">
+        <v>115</v>
       </c>
       <c r="B18" s="56"/>
-      <c r="C18" s="110">
+      <c r="C18" s="97">
         <v>1</v>
       </c>
       <c r="D18" s="58" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="E18" s="57" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F18" s="55"/>
       <c r="G18" s="55"/>
       <c r="H18" s="54"/>
-      <c r="I18" s="63"/>
-      <c r="J18" s="64"/>
+      <c r="I18" s="58" t="s">
+        <v>120</v>
+      </c>
+      <c r="J18" s="105"/>
       <c r="K18" s="3"/>
       <c r="L18" s="3"/>
       <c r="M18" s="3"/>
@@ -2352,25 +2445,27 @@
       <c r="Z18" s="3"/>
     </row>
     <row r="19" spans="1:26" ht="23.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="122" t="s">
-        <v>122</v>
+      <c r="A19" s="104" t="s">
+        <v>116</v>
       </c>
       <c r="B19" s="56"/>
-      <c r="C19" s="110">
+      <c r="C19" s="97">
         <f>C18+1</f>
         <v>2</v>
       </c>
-      <c r="D19" s="60" t="s">
-        <v>77</v>
+      <c r="D19" s="59" t="s">
+        <v>76</v>
       </c>
       <c r="E19" s="57" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F19" s="55"/>
       <c r="G19" s="55"/>
       <c r="H19" s="54"/>
-      <c r="I19" s="59"/>
-      <c r="J19" s="81"/>
+      <c r="I19" s="58" t="s">
+        <v>121</v>
+      </c>
+      <c r="J19" s="105"/>
       <c r="K19" s="3"/>
       <c r="L19" s="3"/>
       <c r="M19" s="3"/>
@@ -2388,26 +2483,28 @@
       <c r="Y19" s="3"/>
       <c r="Z19" s="3"/>
     </row>
-    <row r="20" spans="1:26" ht="23.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="122" t="s">
-        <v>122</v>
+    <row r="20" spans="1:26" ht="26.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.2">
+      <c r="A20" s="104" t="s">
+        <v>116</v>
       </c>
       <c r="B20" s="56"/>
-      <c r="C20" s="110">
+      <c r="C20" s="97">
         <f t="shared" ref="C20:C56" si="0">C19+1</f>
         <v>3</v>
       </c>
-      <c r="D20" s="60" t="s">
-        <v>78</v>
+      <c r="D20" s="59" t="s">
+        <v>77</v>
       </c>
       <c r="E20" s="57" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F20" s="55"/>
       <c r="G20" s="55"/>
       <c r="H20" s="54"/>
-      <c r="I20" s="59"/>
-      <c r="J20" s="81"/>
+      <c r="I20" s="58" t="s">
+        <v>122</v>
+      </c>
+      <c r="J20" s="105"/>
       <c r="K20" s="3"/>
       <c r="L20" s="3"/>
       <c r="M20" s="3"/>
@@ -2426,25 +2523,27 @@
       <c r="Z20" s="3"/>
     </row>
     <row r="21" spans="1:26" ht="23.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="122" t="s">
-        <v>122</v>
+      <c r="A21" s="104" t="s">
+        <v>116</v>
       </c>
       <c r="B21" s="56"/>
-      <c r="C21" s="110">
+      <c r="C21" s="97">
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
-      <c r="D21" s="60" t="s">
-        <v>79</v>
+      <c r="D21" s="59" t="s">
+        <v>78</v>
       </c>
       <c r="E21" s="57" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F21" s="55"/>
       <c r="G21" s="55"/>
       <c r="H21" s="54"/>
-      <c r="I21" s="59"/>
-      <c r="J21" s="81"/>
+      <c r="I21" s="58" t="s">
+        <v>123</v>
+      </c>
+      <c r="J21" s="105"/>
       <c r="K21" s="3"/>
       <c r="L21" s="3"/>
       <c r="M21" s="3"/>
@@ -2462,26 +2561,28 @@
       <c r="Y21" s="3"/>
       <c r="Z21" s="3"/>
     </row>
-    <row r="22" spans="1:26" ht="23.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="122" t="s">
-        <v>122</v>
+    <row r="22" spans="1:26" ht="29.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.2">
+      <c r="A22" s="104" t="s">
+        <v>116</v>
       </c>
       <c r="B22" s="56"/>
-      <c r="C22" s="110">
+      <c r="C22" s="97">
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="D22" s="60" t="s">
-        <v>80</v>
+      <c r="D22" s="59" t="s">
+        <v>79</v>
       </c>
       <c r="E22" s="57" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F22" s="55"/>
       <c r="G22" s="55"/>
       <c r="H22" s="54"/>
-      <c r="I22" s="59"/>
-      <c r="J22" s="81"/>
+      <c r="I22" s="58" t="s">
+        <v>124</v>
+      </c>
+      <c r="J22" s="105"/>
       <c r="K22" s="3"/>
       <c r="L22" s="3"/>
       <c r="M22" s="3"/>
@@ -2499,26 +2600,28 @@
       <c r="Y22" s="3"/>
       <c r="Z22" s="3"/>
     </row>
-    <row r="23" spans="1:26" ht="23.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="122" t="s">
-        <v>121</v>
+    <row r="23" spans="1:26" ht="26.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.2">
+      <c r="A23" s="104" t="s">
+        <v>115</v>
       </c>
       <c r="B23" s="56"/>
-      <c r="C23" s="110">
+      <c r="C23" s="97">
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
-      <c r="D23" s="60" t="s">
-        <v>81</v>
+      <c r="D23" s="59" t="s">
+        <v>80</v>
       </c>
       <c r="E23" s="57" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F23" s="55"/>
       <c r="G23" s="55"/>
       <c r="H23" s="54"/>
-      <c r="I23" s="59"/>
-      <c r="J23" s="81"/>
+      <c r="I23" s="58" t="s">
+        <v>125</v>
+      </c>
+      <c r="J23" s="105"/>
       <c r="K23" s="3"/>
       <c r="L23" s="3"/>
       <c r="M23" s="3"/>
@@ -2536,26 +2639,28 @@
       <c r="Y23" s="3"/>
       <c r="Z23" s="3"/>
     </row>
-    <row r="24" spans="1:26" ht="23.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="122" t="s">
-        <v>121</v>
+    <row r="24" spans="1:26" ht="27" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.2">
+      <c r="A24" s="104" t="s">
+        <v>115</v>
       </c>
       <c r="B24" s="56"/>
-      <c r="C24" s="110">
+      <c r="C24" s="97">
         <f t="shared" si="0"/>
         <v>7</v>
       </c>
-      <c r="D24" s="60" t="s">
-        <v>82</v>
+      <c r="D24" s="59" t="s">
+        <v>81</v>
       </c>
       <c r="E24" s="57" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F24" s="55"/>
       <c r="G24" s="55"/>
       <c r="H24" s="54"/>
-      <c r="I24" s="59"/>
-      <c r="J24" s="81"/>
+      <c r="I24" s="58" t="s">
+        <v>126</v>
+      </c>
+      <c r="J24" s="105"/>
       <c r="K24" s="3"/>
       <c r="L24" s="3"/>
       <c r="M24" s="3"/>
@@ -2573,26 +2678,28 @@
       <c r="Y24" s="3"/>
       <c r="Z24" s="3"/>
     </row>
-    <row r="25" spans="1:26" ht="23.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="122" t="s">
-        <v>121</v>
+    <row r="25" spans="1:26" ht="29.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.2">
+      <c r="A25" s="104" t="s">
+        <v>115</v>
       </c>
       <c r="B25" s="56"/>
-      <c r="C25" s="110">
+      <c r="C25" s="97">
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
-      <c r="D25" s="60" t="s">
-        <v>103</v>
+      <c r="D25" s="59" t="s">
+        <v>99</v>
       </c>
       <c r="E25" s="57" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F25" s="55"/>
       <c r="G25" s="55"/>
       <c r="H25" s="54"/>
-      <c r="I25" s="59"/>
-      <c r="J25" s="81"/>
+      <c r="I25" s="58" t="s">
+        <v>127</v>
+      </c>
+      <c r="J25" s="105"/>
       <c r="K25" s="3"/>
       <c r="L25" s="3"/>
       <c r="M25" s="3"/>
@@ -2610,28 +2717,30 @@
       <c r="Y25" s="3"/>
       <c r="Z25" s="3"/>
     </row>
-    <row r="26" spans="1:26" ht="23.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.2">
-      <c r="A26" s="122" t="s">
-        <v>121</v>
+    <row r="26" spans="1:26" ht="30.75" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.2">
+      <c r="A26" s="104" t="s">
+        <v>115</v>
       </c>
       <c r="B26" s="56"/>
-      <c r="C26" s="110">
+      <c r="C26" s="97">
         <f t="shared" si="0"/>
         <v>9</v>
       </c>
-      <c r="D26" s="60" t="s">
-        <v>83</v>
+      <c r="D26" s="59" t="s">
+        <v>82</v>
       </c>
       <c r="E26" s="57"/>
       <c r="F26" s="55"/>
       <c r="G26" s="55" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="H26" s="54"/>
-      <c r="I26" s="59" t="s">
-        <v>98</v>
-      </c>
-      <c r="J26" s="81"/>
+      <c r="I26" s="58" t="s">
+        <v>128</v>
+      </c>
+      <c r="J26" s="105" t="s">
+        <v>129</v>
+      </c>
       <c r="K26" s="3"/>
       <c r="L26" s="3"/>
       <c r="M26" s="3"/>
@@ -2649,28 +2758,28 @@
       <c r="Y26" s="3"/>
       <c r="Z26" s="3"/>
     </row>
-    <row r="27" spans="1:26" ht="23.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.2">
-      <c r="A27" s="122" t="s">
-        <v>121</v>
+    <row r="27" spans="1:26" ht="29.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.2">
+      <c r="A27" s="104" t="s">
+        <v>115</v>
       </c>
       <c r="B27" s="56"/>
-      <c r="C27" s="110">
+      <c r="C27" s="97">
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
-      <c r="D27" s="60" t="s">
-        <v>84</v>
-      </c>
-      <c r="E27" s="57"/>
+      <c r="D27" s="59" t="s">
+        <v>83</v>
+      </c>
+      <c r="E27" s="57" t="s">
+        <v>13</v>
+      </c>
       <c r="F27" s="55"/>
-      <c r="G27" s="55" t="s">
-        <v>14</v>
-      </c>
+      <c r="G27" s="55"/>
       <c r="H27" s="54"/>
-      <c r="I27" s="59" t="s">
-        <v>85</v>
-      </c>
-      <c r="J27" s="81"/>
+      <c r="I27" s="58" t="s">
+        <v>130</v>
+      </c>
+      <c r="J27" s="105"/>
       <c r="K27" s="3"/>
       <c r="L27" s="3"/>
       <c r="M27" s="3"/>
@@ -2688,26 +2797,28 @@
       <c r="Y27" s="3"/>
       <c r="Z27" s="3"/>
     </row>
-    <row r="28" spans="1:26" ht="23.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.2">
-      <c r="A28" s="122" t="s">
-        <v>121</v>
+    <row r="28" spans="1:26" ht="29.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.2">
+      <c r="A28" s="104" t="s">
+        <v>115</v>
       </c>
       <c r="B28" s="56"/>
-      <c r="C28" s="110">
+      <c r="C28" s="97">
         <f t="shared" si="0"/>
         <v>11</v>
       </c>
-      <c r="D28" s="60" t="s">
-        <v>86</v>
+      <c r="D28" s="59" t="s">
+        <v>84</v>
       </c>
       <c r="E28" s="57" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F28" s="55"/>
       <c r="G28" s="55"/>
       <c r="H28" s="54"/>
-      <c r="I28" s="59"/>
-      <c r="J28" s="81"/>
+      <c r="I28" s="58" t="s">
+        <v>131</v>
+      </c>
+      <c r="J28" s="105"/>
       <c r="K28" s="3"/>
       <c r="L28" s="3"/>
       <c r="M28" s="3"/>
@@ -2725,26 +2836,30 @@
       <c r="Y28" s="3"/>
       <c r="Z28" s="3"/>
     </row>
-    <row r="29" spans="1:26" ht="23.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.2">
-      <c r="A29" s="122" t="s">
-        <v>122</v>
+    <row r="29" spans="1:26" ht="53.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.2">
+      <c r="A29" s="104" t="s">
+        <v>116</v>
       </c>
       <c r="B29" s="56"/>
-      <c r="C29" s="110">
+      <c r="C29" s="97">
         <f t="shared" si="0"/>
         <v>12</v>
       </c>
-      <c r="D29" s="60" t="s">
-        <v>87</v>
-      </c>
-      <c r="E29" s="57" t="s">
-        <v>14</v>
-      </c>
+      <c r="D29" s="59" t="s">
+        <v>85</v>
+      </c>
+      <c r="E29" s="57"/>
       <c r="F29" s="55"/>
-      <c r="G29" s="55"/>
+      <c r="G29" s="55" t="s">
+        <v>13</v>
+      </c>
       <c r="H29" s="54"/>
-      <c r="I29" s="59"/>
-      <c r="J29" s="81"/>
+      <c r="I29" s="58" t="s">
+        <v>132</v>
+      </c>
+      <c r="J29" s="105" t="s">
+        <v>133</v>
+      </c>
       <c r="K29" s="3"/>
       <c r="L29" s="3"/>
       <c r="M29" s="3"/>
@@ -2763,25 +2878,27 @@
       <c r="Z29" s="3"/>
     </row>
     <row r="30" spans="1:26" ht="23.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.2">
-      <c r="A30" s="122" t="s">
-        <v>123</v>
+      <c r="A30" s="104" t="s">
+        <v>117</v>
       </c>
       <c r="B30" s="56"/>
-      <c r="C30" s="110">
+      <c r="C30" s="97">
         <f t="shared" si="0"/>
         <v>13</v>
       </c>
-      <c r="D30" s="60" t="s">
-        <v>88</v>
+      <c r="D30" s="59" t="s">
+        <v>86</v>
       </c>
       <c r="E30" s="57" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F30" s="55"/>
       <c r="G30" s="55"/>
       <c r="H30" s="54"/>
-      <c r="I30" s="59"/>
-      <c r="J30" s="81"/>
+      <c r="I30" s="58" t="s">
+        <v>134</v>
+      </c>
+      <c r="J30" s="105"/>
       <c r="K30" s="3"/>
       <c r="L30" s="3"/>
       <c r="M30" s="3"/>
@@ -2800,25 +2917,27 @@
       <c r="Z30" s="3"/>
     </row>
     <row r="31" spans="1:26" ht="23.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.2">
-      <c r="A31" s="122" t="s">
-        <v>122</v>
+      <c r="A31" s="104" t="s">
+        <v>116</v>
       </c>
       <c r="B31" s="56"/>
-      <c r="C31" s="110">
+      <c r="C31" s="97">
         <f t="shared" si="0"/>
         <v>14</v>
       </c>
-      <c r="D31" s="60" t="s">
-        <v>89</v>
+      <c r="D31" s="59" t="s">
+        <v>87</v>
       </c>
       <c r="E31" s="57" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F31" s="55"/>
       <c r="G31" s="55"/>
       <c r="H31" s="54"/>
-      <c r="I31" s="59"/>
-      <c r="J31" s="81"/>
+      <c r="I31" s="58" t="s">
+        <v>135</v>
+      </c>
+      <c r="J31" s="105"/>
       <c r="K31" s="3"/>
       <c r="L31" s="3"/>
       <c r="M31" s="3"/>
@@ -2836,26 +2955,28 @@
       <c r="Y31" s="3"/>
       <c r="Z31" s="3"/>
     </row>
-    <row r="32" spans="1:26" ht="23.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.2">
-      <c r="A32" s="122" t="s">
-        <v>122</v>
+    <row r="32" spans="1:26" ht="29.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.2">
+      <c r="A32" s="104" t="s">
+        <v>116</v>
       </c>
       <c r="B32" s="56"/>
-      <c r="C32" s="110">
+      <c r="C32" s="97">
         <f t="shared" si="0"/>
         <v>15</v>
       </c>
-      <c r="D32" s="60" t="s">
-        <v>90</v>
+      <c r="D32" s="59" t="s">
+        <v>88</v>
       </c>
       <c r="E32" s="57" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F32" s="55"/>
       <c r="G32" s="55"/>
       <c r="H32" s="54"/>
-      <c r="I32" s="59"/>
-      <c r="J32" s="81"/>
+      <c r="I32" s="58" t="s">
+        <v>136</v>
+      </c>
+      <c r="J32" s="105"/>
       <c r="K32" s="3"/>
       <c r="L32" s="3"/>
       <c r="M32" s="3"/>
@@ -2873,26 +2994,28 @@
       <c r="Y32" s="3"/>
       <c r="Z32" s="3"/>
     </row>
-    <row r="33" spans="1:26" ht="23.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.2">
-      <c r="A33" s="122" t="s">
-        <v>121</v>
+    <row r="33" spans="1:26" ht="22.5" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.2">
+      <c r="A33" s="104" t="s">
+        <v>115</v>
       </c>
       <c r="B33" s="56"/>
-      <c r="C33" s="110">
+      <c r="C33" s="97">
         <f t="shared" si="0"/>
         <v>16</v>
       </c>
-      <c r="D33" s="60" t="s">
-        <v>91</v>
+      <c r="D33" s="59" t="s">
+        <v>89</v>
       </c>
       <c r="E33" s="57" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F33" s="55"/>
       <c r="G33" s="55"/>
       <c r="H33" s="54"/>
-      <c r="I33" s="59"/>
-      <c r="J33" s="81"/>
+      <c r="I33" s="58" t="s">
+        <v>137</v>
+      </c>
+      <c r="J33" s="105"/>
       <c r="K33" s="3"/>
       <c r="L33" s="3"/>
       <c r="M33" s="3"/>
@@ -2910,26 +3033,28 @@
       <c r="Y33" s="3"/>
       <c r="Z33" s="3"/>
     </row>
-    <row r="34" spans="1:26" ht="23.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.2">
-      <c r="A34" s="122" t="s">
-        <v>122</v>
+    <row r="34" spans="1:26" ht="27" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.2">
+      <c r="A34" s="104" t="s">
+        <v>116</v>
       </c>
       <c r="B34" s="56"/>
-      <c r="C34" s="110">
+      <c r="C34" s="97">
         <f t="shared" si="0"/>
         <v>17</v>
       </c>
-      <c r="D34" s="60" t="s">
-        <v>94</v>
+      <c r="D34" s="59" t="s">
+        <v>92</v>
       </c>
       <c r="E34" s="57" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F34" s="55"/>
       <c r="G34" s="55"/>
       <c r="H34" s="54"/>
-      <c r="I34" s="59"/>
-      <c r="J34" s="81"/>
+      <c r="I34" s="58" t="s">
+        <v>138</v>
+      </c>
+      <c r="J34" s="105"/>
       <c r="K34" s="3"/>
       <c r="L34" s="3"/>
       <c r="M34" s="3"/>
@@ -2947,26 +3072,28 @@
       <c r="Y34" s="3"/>
       <c r="Z34" s="3"/>
     </row>
-    <row r="35" spans="1:26" ht="37.5" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.2">
-      <c r="A35" s="122" t="s">
-        <v>121</v>
+    <row r="35" spans="1:26" ht="38.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.2">
+      <c r="A35" s="104" t="s">
+        <v>115</v>
       </c>
       <c r="B35" s="56"/>
-      <c r="C35" s="110">
+      <c r="C35" s="97">
         <f t="shared" si="0"/>
         <v>18</v>
       </c>
-      <c r="D35" s="60" t="s">
-        <v>95</v>
+      <c r="D35" s="59" t="s">
+        <v>93</v>
       </c>
       <c r="E35" s="57" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F35" s="55"/>
       <c r="G35" s="55"/>
       <c r="H35" s="54"/>
-      <c r="I35" s="59"/>
-      <c r="J35" s="81"/>
+      <c r="I35" s="58" t="s">
+        <v>139</v>
+      </c>
+      <c r="J35" s="105"/>
       <c r="K35" s="3"/>
       <c r="L35" s="3"/>
       <c r="M35" s="3"/>
@@ -2984,26 +3111,28 @@
       <c r="Y35" s="3"/>
       <c r="Z35" s="3"/>
     </row>
-    <row r="36" spans="1:26" ht="23.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.2">
-      <c r="A36" s="122" t="s">
-        <v>121</v>
+    <row r="36" spans="1:26" ht="27.75" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.2">
+      <c r="A36" s="104" t="s">
+        <v>115</v>
       </c>
       <c r="B36" s="56"/>
-      <c r="C36" s="110">
+      <c r="C36" s="97">
         <f t="shared" si="0"/>
         <v>19</v>
       </c>
-      <c r="D36" s="60" t="s">
-        <v>92</v>
+      <c r="D36" s="59" t="s">
+        <v>90</v>
       </c>
       <c r="E36" s="57" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F36" s="55"/>
       <c r="G36" s="55"/>
       <c r="H36" s="54"/>
-      <c r="I36" s="59"/>
-      <c r="J36" s="81"/>
+      <c r="I36" s="58" t="s">
+        <v>139</v>
+      </c>
+      <c r="J36" s="105"/>
       <c r="K36" s="3"/>
       <c r="L36" s="3"/>
       <c r="M36" s="3"/>
@@ -3021,26 +3150,28 @@
       <c r="Y36" s="3"/>
       <c r="Z36" s="3"/>
     </row>
-    <row r="37" spans="1:26" ht="23.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.2">
-      <c r="A37" s="122" t="s">
-        <v>121</v>
+    <row r="37" spans="1:26" ht="29.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.2">
+      <c r="A37" s="104" t="s">
+        <v>115</v>
       </c>
       <c r="B37" s="56"/>
-      <c r="C37" s="110">
+      <c r="C37" s="97">
         <f t="shared" si="0"/>
         <v>20</v>
       </c>
-      <c r="D37" s="60" t="s">
-        <v>93</v>
+      <c r="D37" s="59" t="s">
+        <v>91</v>
       </c>
       <c r="E37" s="57" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F37" s="55"/>
       <c r="G37" s="55"/>
       <c r="H37" s="54"/>
-      <c r="I37" s="59"/>
-      <c r="J37" s="81"/>
+      <c r="I37" s="58" t="s">
+        <v>139</v>
+      </c>
+      <c r="J37" s="105"/>
       <c r="K37" s="3"/>
       <c r="L37" s="3"/>
       <c r="M37" s="3"/>
@@ -3058,26 +3189,28 @@
       <c r="Y37" s="3"/>
       <c r="Z37" s="3"/>
     </row>
-    <row r="38" spans="1:26" ht="23.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.2">
-      <c r="A38" s="122" t="s">
-        <v>121</v>
+    <row r="38" spans="1:26" ht="29.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.2">
+      <c r="A38" s="104" t="s">
+        <v>115</v>
       </c>
       <c r="B38" s="56"/>
-      <c r="C38" s="110">
+      <c r="C38" s="97">
         <f t="shared" si="0"/>
         <v>21</v>
       </c>
-      <c r="D38" s="60" t="s">
-        <v>96</v>
+      <c r="D38" s="59" t="s">
+        <v>94</v>
       </c>
       <c r="E38" s="57" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F38" s="55"/>
       <c r="G38" s="55"/>
       <c r="H38" s="54"/>
-      <c r="I38" s="59"/>
-      <c r="J38" s="81"/>
+      <c r="I38" s="58" t="s">
+        <v>139</v>
+      </c>
+      <c r="J38" s="105"/>
       <c r="K38" s="3"/>
       <c r="L38" s="3"/>
       <c r="M38" s="3"/>
@@ -3096,25 +3229,27 @@
       <c r="Z38" s="3"/>
     </row>
     <row r="39" spans="1:26" ht="23.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.2">
-      <c r="A39" s="122" t="s">
-        <v>121</v>
+      <c r="A39" s="104" t="s">
+        <v>115</v>
       </c>
       <c r="B39" s="56"/>
-      <c r="C39" s="110">
+      <c r="C39" s="97">
         <f t="shared" si="0"/>
         <v>22</v>
       </c>
-      <c r="D39" s="60" t="s">
-        <v>97</v>
+      <c r="D39" s="59" t="s">
+        <v>95</v>
       </c>
       <c r="E39" s="57" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F39" s="55"/>
       <c r="G39" s="55"/>
       <c r="H39" s="54"/>
-      <c r="I39" s="59"/>
-      <c r="J39" s="81"/>
+      <c r="I39" s="58" t="s">
+        <v>140</v>
+      </c>
+      <c r="J39" s="105"/>
       <c r="K39" s="3"/>
       <c r="L39" s="3"/>
       <c r="M39" s="3"/>
@@ -3133,23 +3268,23 @@
       <c r="Z39" s="3"/>
     </row>
     <row r="40" spans="1:26" ht="23.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.2">
-      <c r="A40" s="122"/>
+      <c r="A40" s="104"/>
       <c r="B40" s="56"/>
-      <c r="C40" s="110">
+      <c r="C40" s="97">
         <f t="shared" si="0"/>
         <v>23</v>
       </c>
-      <c r="D40" s="60" t="s">
-        <v>105</v>
+      <c r="D40" s="59" t="s">
+        <v>101</v>
       </c>
       <c r="E40" s="57"/>
       <c r="F40" s="55"/>
       <c r="G40" s="55"/>
       <c r="H40" s="54" t="s">
-        <v>14</v>
-      </c>
-      <c r="I40" s="59"/>
-      <c r="J40" s="81"/>
+        <v>13</v>
+      </c>
+      <c r="I40" s="58"/>
+      <c r="J40" s="105"/>
       <c r="K40" s="3"/>
       <c r="L40" s="3"/>
       <c r="M40" s="3"/>
@@ -3167,26 +3302,28 @@
       <c r="Y40" s="3"/>
       <c r="Z40" s="3"/>
     </row>
-    <row r="41" spans="1:26" ht="35.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.2">
-      <c r="A41" s="122" t="s">
-        <v>121</v>
+    <row r="41" spans="1:26" ht="40.5" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.2">
+      <c r="A41" s="104" t="s">
+        <v>115</v>
       </c>
       <c r="B41" s="56"/>
-      <c r="C41" s="110">
+      <c r="C41" s="97">
         <f t="shared" si="0"/>
         <v>24</v>
       </c>
-      <c r="D41" s="60" t="s">
-        <v>110</v>
+      <c r="D41" s="59" t="s">
+        <v>106</v>
       </c>
       <c r="E41" s="57" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F41" s="55"/>
       <c r="G41" s="55"/>
       <c r="H41" s="54"/>
-      <c r="I41" s="59"/>
-      <c r="J41" s="81"/>
+      <c r="I41" s="58" t="s">
+        <v>139</v>
+      </c>
+      <c r="J41" s="105"/>
       <c r="K41" s="3"/>
       <c r="L41" s="3"/>
       <c r="M41" s="3"/>
@@ -3205,23 +3342,23 @@
       <c r="Z41" s="3"/>
     </row>
     <row r="42" spans="1:26" ht="23.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.2">
-      <c r="A42" s="122"/>
+      <c r="A42" s="104"/>
       <c r="B42" s="56"/>
-      <c r="C42" s="110">
+      <c r="C42" s="97">
         <f t="shared" si="0"/>
         <v>25</v>
       </c>
-      <c r="D42" s="60" t="s">
-        <v>112</v>
+      <c r="D42" s="59" t="s">
+        <v>108</v>
       </c>
       <c r="E42" s="57"/>
       <c r="F42" s="55"/>
       <c r="G42" s="55"/>
       <c r="H42" s="54" t="s">
-        <v>14</v>
-      </c>
-      <c r="I42" s="59"/>
-      <c r="J42" s="81"/>
+        <v>13</v>
+      </c>
+      <c r="I42" s="58"/>
+      <c r="J42" s="105"/>
       <c r="K42" s="3"/>
       <c r="L42" s="3"/>
       <c r="M42" s="3"/>
@@ -3239,26 +3376,28 @@
       <c r="Y42" s="3"/>
       <c r="Z42" s="3"/>
     </row>
-    <row r="43" spans="1:26" ht="23.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.2">
-      <c r="A43" s="122" t="s">
-        <v>121</v>
+    <row r="43" spans="1:26" ht="50.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.2">
+      <c r="A43" s="104" t="s">
+        <v>115</v>
       </c>
       <c r="B43" s="56"/>
-      <c r="C43" s="110">
+      <c r="C43" s="97">
         <f t="shared" si="0"/>
         <v>26</v>
       </c>
-      <c r="D43" s="60" t="s">
-        <v>111</v>
+      <c r="D43" s="59" t="s">
+        <v>107</v>
       </c>
       <c r="E43" s="57" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F43" s="55"/>
       <c r="G43" s="55"/>
       <c r="H43" s="54"/>
-      <c r="I43" s="59"/>
-      <c r="J43" s="81"/>
+      <c r="I43" s="58" t="s">
+        <v>141</v>
+      </c>
+      <c r="J43" s="105"/>
       <c r="K43" s="3"/>
       <c r="L43" s="3"/>
       <c r="M43" s="3"/>
@@ -3277,23 +3416,23 @@
       <c r="Z43" s="3"/>
     </row>
     <row r="44" spans="1:26" ht="23.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.2">
-      <c r="A44" s="122"/>
+      <c r="A44" s="104"/>
       <c r="B44" s="56"/>
-      <c r="C44" s="110">
+      <c r="C44" s="97">
         <f t="shared" si="0"/>
         <v>27</v>
       </c>
-      <c r="D44" s="60" t="s">
-        <v>104</v>
+      <c r="D44" s="59" t="s">
+        <v>100</v>
       </c>
       <c r="E44" s="57"/>
       <c r="F44" s="55"/>
       <c r="G44" s="55"/>
       <c r="H44" s="54" t="s">
-        <v>14</v>
-      </c>
-      <c r="I44" s="59"/>
-      <c r="J44" s="81"/>
+        <v>13</v>
+      </c>
+      <c r="I44" s="58"/>
+      <c r="J44" s="105"/>
       <c r="K44" s="3"/>
       <c r="L44" s="3"/>
       <c r="M44" s="3"/>
@@ -3311,28 +3450,30 @@
       <c r="Y44" s="3"/>
       <c r="Z44" s="3"/>
     </row>
-    <row r="45" spans="1:26" ht="23.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.2">
-      <c r="A45" s="122" t="s">
-        <v>122</v>
+    <row r="45" spans="1:26" ht="27" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.2">
+      <c r="A45" s="104" t="s">
+        <v>116</v>
       </c>
       <c r="B45" s="56"/>
-      <c r="C45" s="110">
+      <c r="C45" s="97">
         <f t="shared" si="0"/>
         <v>28</v>
       </c>
-      <c r="D45" s="60" t="s">
-        <v>99</v>
-      </c>
-      <c r="E45" s="57" t="s">
-        <v>14</v>
-      </c>
+      <c r="D45" s="59" t="s">
+        <v>96</v>
+      </c>
+      <c r="E45" s="57"/>
       <c r="F45" s="55"/>
-      <c r="G45" s="55"/>
+      <c r="G45" s="55" t="s">
+        <v>13</v>
+      </c>
       <c r="H45" s="54"/>
-      <c r="I45" s="112" t="s">
-        <v>100</v>
-      </c>
-      <c r="J45" s="113"/>
+      <c r="I45" s="58" t="s">
+        <v>142</v>
+      </c>
+      <c r="J45" s="58" t="s">
+        <v>143</v>
+      </c>
       <c r="K45" s="3"/>
       <c r="L45" s="3"/>
       <c r="M45" s="3"/>
@@ -3350,24 +3491,28 @@
       <c r="Y45" s="3"/>
       <c r="Z45" s="3"/>
     </row>
-    <row r="46" spans="1:26" ht="23.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.2">
-      <c r="A46" s="122" t="s">
-        <v>122</v>
+    <row r="46" spans="1:26" ht="28.5" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.2">
+      <c r="A46" s="104" t="s">
+        <v>116</v>
       </c>
       <c r="B46" s="56"/>
-      <c r="C46" s="110">
+      <c r="C46" s="97">
         <f t="shared" si="0"/>
         <v>29</v>
       </c>
-      <c r="D46" s="60" t="s">
-        <v>101</v>
-      </c>
-      <c r="E46" s="57"/>
+      <c r="D46" s="59" t="s">
+        <v>97</v>
+      </c>
+      <c r="E46" s="57" t="s">
+        <v>13</v>
+      </c>
       <c r="F46" s="55"/>
       <c r="G46" s="55"/>
       <c r="H46" s="54"/>
-      <c r="I46" s="59"/>
-      <c r="J46" s="81"/>
+      <c r="I46" s="58" t="s">
+        <v>124</v>
+      </c>
+      <c r="J46" s="105"/>
       <c r="K46" s="3"/>
       <c r="L46" s="3"/>
       <c r="M46" s="3"/>
@@ -3385,24 +3530,28 @@
       <c r="Y46" s="3"/>
       <c r="Z46" s="3"/>
     </row>
-    <row r="47" spans="1:26" ht="23.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.2">
-      <c r="A47" s="122" t="s">
-        <v>122</v>
+    <row r="47" spans="1:26" ht="27" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.2">
+      <c r="A47" s="104" t="s">
+        <v>116</v>
       </c>
       <c r="B47" s="56"/>
-      <c r="C47" s="110">
+      <c r="C47" s="97">
         <f t="shared" si="0"/>
         <v>30</v>
       </c>
-      <c r="D47" s="60" t="s">
-        <v>108</v>
-      </c>
-      <c r="E47" s="57"/>
+      <c r="D47" s="59" t="s">
+        <v>104</v>
+      </c>
+      <c r="E47" s="57" t="s">
+        <v>13</v>
+      </c>
       <c r="F47" s="55"/>
       <c r="G47" s="55"/>
       <c r="H47" s="54"/>
-      <c r="I47" s="59"/>
-      <c r="J47" s="81"/>
+      <c r="I47" s="58" t="s">
+        <v>144</v>
+      </c>
+      <c r="J47" s="105"/>
       <c r="K47" s="3"/>
       <c r="L47" s="3"/>
       <c r="M47" s="3"/>
@@ -3420,24 +3569,28 @@
       <c r="Y47" s="3"/>
       <c r="Z47" s="3"/>
     </row>
-    <row r="48" spans="1:26" ht="23.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.2">
-      <c r="A48" s="122" t="s">
-        <v>121</v>
+    <row r="48" spans="1:26" ht="27.75" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.2">
+      <c r="A48" s="104" t="s">
+        <v>115</v>
       </c>
       <c r="B48" s="56"/>
-      <c r="C48" s="110">
+      <c r="C48" s="97">
         <f t="shared" si="0"/>
         <v>31</v>
       </c>
-      <c r="D48" s="60" t="s">
-        <v>102</v>
-      </c>
-      <c r="E48" s="57"/>
+      <c r="D48" s="59" t="s">
+        <v>98</v>
+      </c>
+      <c r="E48" s="57" t="s">
+        <v>13</v>
+      </c>
       <c r="F48" s="55"/>
       <c r="G48" s="55"/>
       <c r="H48" s="54"/>
-      <c r="I48" s="59"/>
-      <c r="J48" s="81"/>
+      <c r="I48" s="58" t="s">
+        <v>145</v>
+      </c>
+      <c r="J48" s="105"/>
       <c r="K48" s="3"/>
       <c r="L48" s="3"/>
       <c r="M48" s="3"/>
@@ -3456,23 +3609,23 @@
       <c r="Z48" s="3"/>
     </row>
     <row r="49" spans="1:26" ht="23.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.2">
-      <c r="A49" s="122"/>
+      <c r="A49" s="104"/>
       <c r="B49" s="56"/>
-      <c r="C49" s="110">
+      <c r="C49" s="97">
         <f t="shared" si="0"/>
         <v>32</v>
       </c>
-      <c r="D49" s="60" t="s">
-        <v>106</v>
+      <c r="D49" s="59" t="s">
+        <v>102</v>
       </c>
       <c r="E49" s="57"/>
       <c r="F49" s="55"/>
       <c r="G49" s="55"/>
       <c r="H49" s="54" t="s">
-        <v>14</v>
-      </c>
-      <c r="I49" s="59"/>
-      <c r="J49" s="81"/>
+        <v>13</v>
+      </c>
+      <c r="I49" s="58"/>
+      <c r="J49" s="105"/>
       <c r="K49" s="3"/>
       <c r="L49" s="3"/>
       <c r="M49" s="3"/>
@@ -3490,26 +3643,28 @@
       <c r="Y49" s="3"/>
       <c r="Z49" s="3"/>
     </row>
-    <row r="50" spans="1:26" ht="23.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.2">
-      <c r="A50" s="122" t="s">
-        <v>121</v>
+    <row r="50" spans="1:26" ht="40.5" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.2">
+      <c r="A50" s="104" t="s">
+        <v>115</v>
       </c>
       <c r="B50" s="56"/>
-      <c r="C50" s="110">
+      <c r="C50" s="97">
         <f t="shared" si="0"/>
         <v>33</v>
       </c>
-      <c r="D50" s="60" t="s">
-        <v>107</v>
+      <c r="D50" s="59" t="s">
+        <v>103</v>
       </c>
       <c r="E50" s="57" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F50" s="55"/>
       <c r="G50" s="55"/>
       <c r="H50" s="54"/>
-      <c r="I50" s="59"/>
-      <c r="J50" s="81"/>
+      <c r="I50" s="58" t="s">
+        <v>146</v>
+      </c>
+      <c r="J50" s="105"/>
       <c r="K50" s="3"/>
       <c r="L50" s="3"/>
       <c r="M50" s="3"/>
@@ -3527,26 +3682,28 @@
       <c r="Y50" s="3"/>
       <c r="Z50" s="3"/>
     </row>
-    <row r="51" spans="1:26" ht="23.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.2">
-      <c r="A51" s="122" t="s">
-        <v>121</v>
+    <row r="51" spans="1:26" ht="40.5" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.2">
+      <c r="A51" s="104" t="s">
+        <v>115</v>
       </c>
       <c r="B51" s="56"/>
-      <c r="C51" s="110">
+      <c r="C51" s="97">
         <f t="shared" si="0"/>
         <v>34</v>
       </c>
-      <c r="D51" s="60" t="s">
-        <v>109</v>
+      <c r="D51" s="59" t="s">
+        <v>105</v>
       </c>
       <c r="E51" s="57" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F51" s="55"/>
       <c r="G51" s="55"/>
       <c r="H51" s="54"/>
-      <c r="I51" s="59"/>
-      <c r="J51" s="81"/>
+      <c r="I51" s="58" t="s">
+        <v>146</v>
+      </c>
+      <c r="J51" s="105"/>
       <c r="K51" s="3"/>
       <c r="L51" s="3"/>
       <c r="M51" s="3"/>
@@ -3564,28 +3721,28 @@
       <c r="Y51" s="3"/>
       <c r="Z51" s="3"/>
     </row>
-    <row r="52" spans="1:26" ht="23.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.2">
-      <c r="A52" s="122" t="s">
-        <v>121</v>
+    <row r="52" spans="1:26" ht="38.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.2">
+      <c r="A52" s="104" t="s">
+        <v>115</v>
       </c>
       <c r="B52" s="56"/>
-      <c r="C52" s="110">
+      <c r="C52" s="97">
         <f t="shared" si="0"/>
         <v>35</v>
       </c>
-      <c r="D52" s="60" t="s">
-        <v>113</v>
-      </c>
-      <c r="E52" s="57"/>
+      <c r="D52" s="59" t="s">
+        <v>109</v>
+      </c>
+      <c r="E52" s="57" t="s">
+        <v>13</v>
+      </c>
       <c r="F52" s="55"/>
-      <c r="G52" s="55" t="s">
-        <v>14</v>
-      </c>
+      <c r="G52" s="55"/>
       <c r="H52" s="54"/>
-      <c r="I52" s="112" t="s">
-        <v>114</v>
-      </c>
-      <c r="J52" s="113"/>
+      <c r="I52" s="58" t="s">
+        <v>147</v>
+      </c>
+      <c r="J52" s="58"/>
       <c r="K52" s="3"/>
       <c r="L52" s="3"/>
       <c r="M52" s="3"/>
@@ -3603,26 +3760,28 @@
       <c r="Y52" s="3"/>
       <c r="Z52" s="3"/>
     </row>
-    <row r="53" spans="1:26" ht="23.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.2">
-      <c r="A53" s="122" t="s">
-        <v>121</v>
+    <row r="53" spans="1:26" ht="52.5" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.2">
+      <c r="A53" s="104" t="s">
+        <v>115</v>
       </c>
       <c r="B53" s="56"/>
-      <c r="C53" s="110">
+      <c r="C53" s="97">
         <f t="shared" si="0"/>
         <v>36</v>
       </c>
-      <c r="D53" s="60" t="s">
-        <v>115</v>
+      <c r="D53" s="59" t="s">
+        <v>110</v>
       </c>
       <c r="E53" s="57" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F53" s="55"/>
       <c r="G53" s="55"/>
       <c r="H53" s="54"/>
-      <c r="I53" s="59"/>
-      <c r="J53" s="81"/>
+      <c r="I53" s="58" t="s">
+        <v>148</v>
+      </c>
+      <c r="J53" s="105"/>
       <c r="K53" s="3"/>
       <c r="L53" s="3"/>
       <c r="M53" s="3"/>
@@ -3640,26 +3799,24 @@
       <c r="Y53" s="3"/>
       <c r="Z53" s="3"/>
     </row>
-    <row r="54" spans="1:26" ht="45.75" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.2">
-      <c r="A54" s="122"/>
+    <row r="54" spans="1:26" ht="21" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.2">
+      <c r="A54" s="104"/>
       <c r="B54" s="56"/>
-      <c r="C54" s="110">
+      <c r="C54" s="97">
         <f t="shared" si="0"/>
         <v>37</v>
       </c>
-      <c r="D54" s="60" t="s">
-        <v>116</v>
+      <c r="D54" s="59" t="s">
+        <v>111</v>
       </c>
       <c r="E54" s="57"/>
       <c r="F54" s="55"/>
       <c r="G54" s="55"/>
       <c r="H54" s="54" t="s">
-        <v>14</v>
-      </c>
-      <c r="I54" s="112" t="s">
-        <v>117</v>
-      </c>
-      <c r="J54" s="113"/>
+        <v>13</v>
+      </c>
+      <c r="I54" s="58"/>
+      <c r="J54" s="58"/>
       <c r="K54" s="3"/>
       <c r="L54" s="3"/>
       <c r="M54" s="3"/>
@@ -3677,26 +3834,28 @@
       <c r="Y54" s="3"/>
       <c r="Z54" s="3"/>
     </row>
-    <row r="55" spans="1:26" ht="23.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.2">
-      <c r="A55" s="122" t="s">
-        <v>122</v>
+    <row r="55" spans="1:26" ht="29.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.2">
+      <c r="A55" s="104" t="s">
+        <v>116</v>
       </c>
       <c r="B55" s="56"/>
-      <c r="C55" s="110">
+      <c r="C55" s="97">
         <f t="shared" si="0"/>
         <v>38</v>
       </c>
-      <c r="D55" s="60" t="s">
-        <v>118</v>
+      <c r="D55" s="59" t="s">
+        <v>112</v>
       </c>
       <c r="E55" s="57" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F55" s="55"/>
       <c r="G55" s="55"/>
       <c r="H55" s="54"/>
-      <c r="I55" s="59"/>
-      <c r="J55" s="81"/>
+      <c r="I55" s="58" t="s">
+        <v>149</v>
+      </c>
+      <c r="J55" s="105"/>
       <c r="K55" s="3"/>
       <c r="L55" s="3"/>
       <c r="M55" s="3"/>
@@ -3714,26 +3873,30 @@
       <c r="Y55" s="3"/>
       <c r="Z55" s="3"/>
     </row>
-    <row r="56" spans="1:26" ht="23.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.2">
-      <c r="A56" s="122" t="s">
-        <v>123</v>
+    <row r="56" spans="1:26" ht="30" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.2">
+      <c r="A56" s="104" t="s">
+        <v>117</v>
       </c>
       <c r="B56" s="56"/>
-      <c r="C56" s="110">
+      <c r="C56" s="97">
         <f t="shared" si="0"/>
         <v>39</v>
       </c>
-      <c r="D56" s="60" t="s">
-        <v>119</v>
-      </c>
-      <c r="E56" s="54" t="s">
-        <v>14</v>
-      </c>
+      <c r="D56" s="59" t="s">
+        <v>113</v>
+      </c>
+      <c r="E56" s="54"/>
       <c r="F56" s="54"/>
-      <c r="G56" s="54"/>
+      <c r="G56" s="54" t="s">
+        <v>13</v>
+      </c>
       <c r="H56" s="54"/>
-      <c r="I56" s="63"/>
-      <c r="J56" s="64"/>
+      <c r="I56" s="58" t="s">
+        <v>150</v>
+      </c>
+      <c r="J56" s="105" t="s">
+        <v>151</v>
+      </c>
       <c r="K56" s="3"/>
       <c r="L56" s="3"/>
       <c r="M56" s="3"/>
@@ -3754,27 +3917,27 @@
     <row r="57" spans="1:26" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A57" s="3"/>
       <c r="B57" s="3"/>
-      <c r="C57" s="61"/>
-      <c r="D57" s="111" t="s">
-        <v>15</v>
-      </c>
-      <c r="E57" s="80">
+      <c r="C57" s="60"/>
+      <c r="D57" s="98" t="s">
+        <v>14</v>
+      </c>
+      <c r="E57" s="73">
         <f>COUNTA(E18:E56)</f>
-        <v>28</v>
-      </c>
-      <c r="F57" s="80">
+        <v>30</v>
+      </c>
+      <c r="F57" s="73">
         <f>COUNTA(F18:F56)</f>
         <v>0</v>
       </c>
-      <c r="G57" s="80">
+      <c r="G57" s="73">
         <f>COUNTA(G18:G56)</f>
-        <v>3</v>
-      </c>
-      <c r="H57" s="80">
+        <v>4</v>
+      </c>
+      <c r="H57" s="73">
         <f>COUNTA(H18:H56)</f>
         <v>5</v>
       </c>
-      <c r="I57" s="62"/>
+      <c r="I57" s="61"/>
       <c r="J57" s="3"/>
       <c r="K57" s="3"/>
       <c r="L57" s="3"/>
@@ -3825,9 +3988,9 @@
       <c r="A59" s="3"/>
       <c r="B59" s="3"/>
       <c r="C59" s="3"/>
-      <c r="D59" s="62"/>
-      <c r="E59" s="116" t="s">
-        <v>16</v>
+      <c r="D59" s="61"/>
+      <c r="E59" s="101" t="s">
+        <v>15</v>
       </c>
       <c r="F59" s="5"/>
       <c r="G59" s="5"/>
@@ -3854,11 +4017,11 @@
     <row r="60" spans="1:26" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A60" s="3"/>
       <c r="B60" s="3"/>
-      <c r="C60" s="65"/>
-      <c r="D60" s="114" t="s">
-        <v>17</v>
-      </c>
-      <c r="E60" s="117">
+      <c r="C60" s="62"/>
+      <c r="D60" s="99" t="s">
+        <v>16</v>
+      </c>
+      <c r="E60" s="102">
         <f>IF(E57+F57=0,0,E57/(E57+F57))</f>
         <v>1</v>
       </c>
@@ -3887,11 +4050,11 @@
     <row r="61" spans="1:26" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A61" s="3"/>
       <c r="B61" s="3"/>
-      <c r="C61" s="65"/>
-      <c r="D61" s="114" t="s">
-        <v>18</v>
-      </c>
-      <c r="E61" s="118">
+      <c r="C61" s="62"/>
+      <c r="D61" s="99" t="s">
+        <v>17</v>
+      </c>
+      <c r="E61" s="103">
         <f>IF(E57+F57=0,0,F57/(F57+E57))</f>
         <v>0</v>
       </c>
@@ -3920,13 +4083,13 @@
     <row r="62" spans="1:26" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A62" s="3"/>
       <c r="B62" s="3"/>
-      <c r="C62" s="66"/>
-      <c r="D62" s="115" t="s">
-        <v>19</v>
-      </c>
-      <c r="E62" s="118">
+      <c r="C62" s="63"/>
+      <c r="D62" s="100" t="s">
+        <v>18</v>
+      </c>
+      <c r="E62" s="103">
         <f>IF(E57+G57=0,0,G57/(G57+E57))</f>
-        <v>9.6774193548387094E-2</v>
+        <v>0.11764705882352941</v>
       </c>
       <c r="F62" s="7"/>
       <c r="G62" s="7"/>
@@ -3981,14 +4144,14 @@
     <row r="64" spans="1:26" ht="3" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A64" s="3"/>
       <c r="B64" s="3"/>
-      <c r="C64" s="99"/>
-      <c r="D64" s="100"/>
-      <c r="E64" s="100"/>
-      <c r="F64" s="100"/>
-      <c r="G64" s="100"/>
-      <c r="H64" s="100"/>
-      <c r="I64" s="100"/>
-      <c r="J64" s="101"/>
+      <c r="C64" s="91"/>
+      <c r="D64" s="92"/>
+      <c r="E64" s="92"/>
+      <c r="F64" s="92"/>
+      <c r="G64" s="92"/>
+      <c r="H64" s="92"/>
+      <c r="I64" s="92"/>
+      <c r="J64" s="93"/>
       <c r="K64" s="3"/>
       <c r="L64" s="3"/>
       <c r="M64" s="3"/>
@@ -4009,18 +4172,18 @@
     <row r="65" spans="1:26" ht="26.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A65" s="3"/>
       <c r="B65" s="3"/>
-      <c r="C65" s="102"/>
-      <c r="D65" s="103" t="s">
-        <v>20</v>
-      </c>
-      <c r="E65" s="119" t="s">
-        <v>120</v>
-      </c>
-      <c r="F65" s="120"/>
-      <c r="G65" s="120"/>
-      <c r="H65" s="120"/>
-      <c r="I65" s="121"/>
-      <c r="J65" s="104"/>
+      <c r="C65" s="94"/>
+      <c r="D65" s="95" t="s">
+        <v>19</v>
+      </c>
+      <c r="E65" s="106" t="s">
+        <v>114</v>
+      </c>
+      <c r="F65" s="107"/>
+      <c r="G65" s="107"/>
+      <c r="H65" s="107"/>
+      <c r="I65" s="108"/>
+      <c r="J65" s="96"/>
       <c r="K65" s="3"/>
       <c r="L65" s="3"/>
       <c r="M65" s="3"/>
@@ -4042,7 +4205,7 @@
       <c r="A66" s="3"/>
       <c r="B66" s="3"/>
       <c r="C66" s="8" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="F66" s="8"/>
       <c r="G66" s="8"/>
@@ -4068,10 +4231,10 @@
       <c r="A67" s="3"/>
       <c r="B67" s="9"/>
       <c r="C67" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="D67" s="10" t="s">
         <v>22</v>
-      </c>
-      <c r="D67" s="10" t="s">
-        <v>23</v>
       </c>
       <c r="E67" s="9"/>
       <c r="F67" s="8"/>
@@ -31257,25 +31420,18 @@
       <c r="Z1037" s="3"/>
     </row>
   </sheetData>
-  <mergeCells count="12">
-    <mergeCell ref="I56:J56"/>
+  <mergeCells count="8">
+    <mergeCell ref="J15:J16"/>
     <mergeCell ref="E65:I65"/>
     <mergeCell ref="E4:I4"/>
     <mergeCell ref="E6:I6"/>
     <mergeCell ref="E8:F8"/>
     <mergeCell ref="E10:I10"/>
     <mergeCell ref="E15:H15"/>
-    <mergeCell ref="I15:J16"/>
-    <mergeCell ref="I18:J18"/>
-    <mergeCell ref="I45:J45"/>
-    <mergeCell ref="I52:J52"/>
-    <mergeCell ref="I54:J54"/>
+    <mergeCell ref="I15:I16"/>
   </mergeCells>
-  <pageMargins left="0.23622047244094491" right="0.23622047244094491" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
-  <pageSetup paperSize="9" scale="59" orientation="portrait" r:id="rId1"/>
-  <headerFooter>
-    <oddFooter>&amp;L&amp;F&amp;RPágina &amp;P de</oddFooter>
-  </headerFooter>
+  <pageMargins left="0.23622047244094491" right="0.23622047244094491" top="0.39370078740157483" bottom="0.19685039370078741" header="0.31496062992125984" footer="0.31496062992125984"/>
+  <pageSetup paperSize="9" scale="55" orientation="portrait" r:id="rId1"/>
   <drawing r:id="rId2"/>
 </worksheet>
 </file>
@@ -31304,28 +31460,28 @@
   <sheetData>
     <row r="1" spans="1:8" ht="26.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="B1" s="12" t="s">
         <v>24</v>
       </c>
-      <c r="B1" s="12" t="s">
+      <c r="C1" s="12" t="s">
         <v>25</v>
       </c>
-      <c r="C1" s="12" t="s">
+      <c r="D1" s="12" t="s">
         <v>26</v>
       </c>
-      <c r="D1" s="12" t="s">
+      <c r="E1" s="12" t="s">
         <v>27</v>
       </c>
-      <c r="E1" s="12" t="s">
+      <c r="F1" s="12" t="s">
         <v>28</v>
       </c>
-      <c r="F1" s="12" t="s">
+      <c r="G1" s="12" t="s">
         <v>29</v>
       </c>
-      <c r="G1" s="12" t="s">
+      <c r="H1" s="12" t="s">
         <v>30</v>
-      </c>
-      <c r="H1" s="12" t="s">
-        <v>31</v>
       </c>
     </row>
     <row r="2" spans="1:8" ht="21" customHeight="1" x14ac:dyDescent="0.2">
@@ -32387,10 +32543,10 @@
         <v>CodPregunta</v>
       </c>
       <c r="B1" s="17" t="s">
+        <v>31</v>
+      </c>
+      <c r="C1" s="17" t="s">
         <v>32</v>
-      </c>
-      <c r="C1" s="17" t="s">
-        <v>33</v>
       </c>
       <c r="D1" s="17" t="str">
         <f>Preg_Respuestas!D1</f>
@@ -32406,7 +32562,7 @@
         <v>1</v>
       </c>
       <c r="C2" s="18" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D2" s="18" t="e">
         <f>Preg_Respuestas!D2</f>
@@ -32422,7 +32578,7 @@
         <v>1</v>
       </c>
       <c r="C3" s="18" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D3" s="18" t="e">
         <f>Preg_Respuestas!D3</f>
@@ -32438,7 +32594,7 @@
         <v>1</v>
       </c>
       <c r="C4" s="18" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D4" s="18" t="e">
         <f>Preg_Respuestas!D4</f>
@@ -32454,7 +32610,7 @@
         <v>1</v>
       </c>
       <c r="C5" s="18" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D5" s="18" t="e">
         <f>Preg_Respuestas!D5</f>
@@ -32470,7 +32626,7 @@
         <v>1</v>
       </c>
       <c r="C6" s="18" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D6" s="18" t="e">
         <f>Preg_Respuestas!D6</f>
@@ -32486,7 +32642,7 @@
         <v>1</v>
       </c>
       <c r="C7" s="18" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D7" s="18" t="e">
         <f>Preg_Respuestas!D7</f>
@@ -32502,7 +32658,7 @@
         <v>1</v>
       </c>
       <c r="C8" s="18" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D8" s="18" t="e">
         <f>Preg_Respuestas!D8</f>
@@ -32518,7 +32674,7 @@
         <v>1</v>
       </c>
       <c r="C9" s="18" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D9" s="18" t="e">
         <f>Preg_Respuestas!D9</f>
@@ -32534,7 +32690,7 @@
         <v>1</v>
       </c>
       <c r="C10" s="18" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D10" s="18" t="e">
         <f>Preg_Respuestas!D10</f>
@@ -32550,7 +32706,7 @@
         <v>1</v>
       </c>
       <c r="C11" s="18" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D11" s="18" t="e">
         <f>Preg_Respuestas!D11</f>
@@ -32566,7 +32722,7 @@
         <v>2</v>
       </c>
       <c r="C12" s="18" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D12" s="18" t="e">
         <f>Preg_Respuestas!D12</f>
@@ -32582,7 +32738,7 @@
         <v>2</v>
       </c>
       <c r="C13" s="18" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D13" s="18" t="e">
         <f>Preg_Respuestas!D13</f>
@@ -32598,7 +32754,7 @@
         <v>3</v>
       </c>
       <c r="C14" s="18" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D14" s="18" t="e">
         <f>Preg_Respuestas!D14</f>
@@ -32614,7 +32770,7 @@
         <v>3</v>
       </c>
       <c r="C15" s="18" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D15" s="18" t="e">
         <f>Preg_Respuestas!D15</f>
@@ -32630,7 +32786,7 @@
         <v>4</v>
       </c>
       <c r="C16" s="18" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D16" s="18" t="e">
         <f>Preg_Respuestas!D16</f>
@@ -32646,7 +32802,7 @@
         <v>4</v>
       </c>
       <c r="C17" s="18" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D17" s="18" t="e">
         <f>Preg_Respuestas!D17</f>
@@ -32662,7 +32818,7 @@
         <v>4</v>
       </c>
       <c r="C18" s="18" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D18" s="18" t="e">
         <f>Preg_Respuestas!D18</f>
@@ -32678,7 +32834,7 @@
         <v>4</v>
       </c>
       <c r="C19" s="18" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D19" s="18" t="e">
         <f>Preg_Respuestas!D19</f>
@@ -32694,7 +32850,7 @@
         <v>4</v>
       </c>
       <c r="C20" s="18" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D20" s="18" t="e">
         <f>Preg_Respuestas!D20</f>
@@ -32710,7 +32866,7 @@
         <v>4</v>
       </c>
       <c r="C21" s="18" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D21" s="18" t="e">
         <f>Preg_Respuestas!D21</f>
@@ -32726,7 +32882,7 @@
         <v>4</v>
       </c>
       <c r="C22" s="18" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D22" s="18" t="e">
         <f>Preg_Respuestas!D22</f>
@@ -32742,7 +32898,7 @@
         <v>4</v>
       </c>
       <c r="C23" s="18" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D23" s="18" t="e">
         <f>Preg_Respuestas!D23</f>
@@ -32758,7 +32914,7 @@
         <v>4</v>
       </c>
       <c r="C24" s="18" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D24" s="18" t="e">
         <f>Preg_Respuestas!D24</f>
@@ -32774,7 +32930,7 @@
         <v>5</v>
       </c>
       <c r="C25" s="18" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D25" s="18" t="e">
         <f>Preg_Respuestas!D25</f>
@@ -32790,7 +32946,7 @@
         <v>5</v>
       </c>
       <c r="C26" s="18" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D26" s="18" t="e">
         <f>Preg_Respuestas!D26</f>
@@ -32806,7 +32962,7 @@
         <v>5</v>
       </c>
       <c r="C27" s="18" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D27" s="18" t="e">
         <f>Preg_Respuestas!D27</f>
@@ -32822,7 +32978,7 @@
         <v>5</v>
       </c>
       <c r="C28" s="18" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D28" s="18" t="e">
         <f>Preg_Respuestas!D28</f>
@@ -32838,7 +32994,7 @@
         <v>5</v>
       </c>
       <c r="C29" s="18" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D29" s="18" t="e">
         <f>Preg_Respuestas!D29</f>
@@ -32854,7 +33010,7 @@
         <v>5</v>
       </c>
       <c r="C30" s="18" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D30" s="18" t="e">
         <f>Preg_Respuestas!D30</f>
@@ -32870,7 +33026,7 @@
         <v>5</v>
       </c>
       <c r="C31" s="18" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D31" s="18" t="e">
         <f>Preg_Respuestas!D31</f>
@@ -32886,7 +33042,7 @@
         <v>6</v>
       </c>
       <c r="C32" s="18" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D32" s="18" t="e">
         <f>Preg_Respuestas!D32</f>
@@ -32902,7 +33058,7 @@
         <v>6</v>
       </c>
       <c r="C33" s="18" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D33" s="18" t="e">
         <f>Preg_Respuestas!D33</f>
@@ -32918,7 +33074,7 @@
         <v>6</v>
       </c>
       <c r="C34" s="18" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D34" s="18" t="e">
         <f>Preg_Respuestas!D34</f>
@@ -32934,7 +33090,7 @@
         <v>6</v>
       </c>
       <c r="C35" s="18" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D35" s="18" t="e">
         <f>Preg_Respuestas!D35</f>
@@ -32950,7 +33106,7 @@
         <v>6</v>
       </c>
       <c r="C36" s="18" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D36" s="18" t="e">
         <f>Preg_Respuestas!D36</f>
@@ -32966,7 +33122,7 @@
         <v>6</v>
       </c>
       <c r="C37" s="18" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D37" s="18" t="e">
         <f>Preg_Respuestas!D37</f>
@@ -32982,7 +33138,7 @@
         <v>6</v>
       </c>
       <c r="C38" s="18" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D38" s="18" t="e">
         <f>Preg_Respuestas!D38</f>
@@ -32998,7 +33154,7 @@
         <v>6</v>
       </c>
       <c r="C39" s="18" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D39" s="18" t="e">
         <f>Preg_Respuestas!D39</f>
@@ -33014,7 +33170,7 @@
         <v>6</v>
       </c>
       <c r="C40" s="18" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D40" s="18" t="e">
         <f>Preg_Respuestas!D40</f>
@@ -33030,7 +33186,7 @@
         <v>6</v>
       </c>
       <c r="C41" s="18" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D41" s="18" t="e">
         <f>Preg_Respuestas!D41</f>
@@ -33046,7 +33202,7 @@
         <v>6</v>
       </c>
       <c r="C42" s="18" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D42" s="18" t="e">
         <f>Preg_Respuestas!D42</f>
@@ -33062,7 +33218,7 @@
         <v>6</v>
       </c>
       <c r="C43" s="18" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D43" s="18" t="e">
         <f>Preg_Respuestas!D43</f>
@@ -33078,7 +33234,7 @@
         <v>6</v>
       </c>
       <c r="C44" s="18" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D44" s="18" t="e">
         <f>Preg_Respuestas!D44</f>
@@ -33094,7 +33250,7 @@
         <v>6</v>
       </c>
       <c r="C45" s="18" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D45" s="18" t="e">
         <f>Preg_Respuestas!D45</f>
@@ -33110,7 +33266,7 @@
         <v>6</v>
       </c>
       <c r="C46" s="18" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D46" s="18" t="e">
         <f>Preg_Respuestas!D46</f>
@@ -33126,7 +33282,7 @@
         <v>7</v>
       </c>
       <c r="C47" s="18" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D47" s="18" t="e">
         <f>Preg_Respuestas!D47</f>
@@ -33142,7 +33298,7 @@
         <v>7</v>
       </c>
       <c r="C48" s="18" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D48" s="18" t="e">
         <f>Preg_Respuestas!D48</f>
@@ -33158,7 +33314,7 @@
         <v>7</v>
       </c>
       <c r="C49" s="18" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D49" s="18" t="e">
         <f>Preg_Respuestas!D49</f>
@@ -33174,7 +33330,7 @@
         <v>7</v>
       </c>
       <c r="C50" s="18" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D50" s="18" t="e">
         <f>Preg_Respuestas!D50</f>
@@ -33190,7 +33346,7 @@
         <v>8</v>
       </c>
       <c r="C51" s="18" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D51" s="18" t="e">
         <f>Preg_Respuestas!D51</f>
@@ -33206,7 +33362,7 @@
         <v>8</v>
       </c>
       <c r="C52" s="18" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D52" s="18" t="e">
         <f>Preg_Respuestas!D52</f>
@@ -33222,7 +33378,7 @@
         <v>8</v>
       </c>
       <c r="C53" s="18" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D53" s="18" t="e">
         <f>Preg_Respuestas!D53</f>
@@ -33238,7 +33394,7 @@
         <v>9</v>
       </c>
       <c r="C54" s="18" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D54" s="18" t="e">
         <f>Preg_Respuestas!D54</f>
@@ -33254,7 +33410,7 @@
         <v>9</v>
       </c>
       <c r="C55" s="18" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D55" s="18" t="e">
         <f>Preg_Respuestas!D55</f>
@@ -33270,7 +33426,7 @@
         <v>9</v>
       </c>
       <c r="C56" s="18" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D56" s="18" t="e">
         <f>Preg_Respuestas!D56</f>
@@ -33286,7 +33442,7 @@
         <v>9</v>
       </c>
       <c r="C57" s="18" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D57" s="18" t="e">
         <f>Preg_Respuestas!D57</f>
@@ -33302,7 +33458,7 @@
         <v>9</v>
       </c>
       <c r="C58" s="18" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D58" s="18" t="e">
         <f>Preg_Respuestas!D58</f>
@@ -33318,7 +33474,7 @@
         <v>9</v>
       </c>
       <c r="C59" s="18" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D59" s="18" t="e">
         <f>Preg_Respuestas!D59</f>
@@ -33334,7 +33490,7 @@
         <v>10</v>
       </c>
       <c r="C60" s="18" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D60" s="18" t="e">
         <f>Preg_Respuestas!D60</f>
@@ -33350,7 +33506,7 @@
         <v>10</v>
       </c>
       <c r="C61" s="18" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D61" s="18" t="e">
         <f>Preg_Respuestas!D61</f>
@@ -33366,7 +33522,7 @@
         <v>10</v>
       </c>
       <c r="C62" s="18" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D62" s="18" t="e">
         <f>Preg_Respuestas!D62</f>
@@ -33382,7 +33538,7 @@
         <v>10</v>
       </c>
       <c r="C63" s="18" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D63" s="18" t="e">
         <f>Preg_Respuestas!D63</f>
@@ -33398,7 +33554,7 @@
         <v>10</v>
       </c>
       <c r="C64" s="18" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D64" s="18" t="e">
         <f>Preg_Respuestas!D64</f>
@@ -33414,7 +33570,7 @@
         <v>11</v>
       </c>
       <c r="C65" s="18" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D65" s="18" t="e">
         <f>Preg_Respuestas!D65</f>
@@ -33430,7 +33586,7 @@
         <v>11</v>
       </c>
       <c r="C66" s="18" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D66" s="18" t="e">
         <f>Preg_Respuestas!D66</f>
@@ -33446,7 +33602,7 @@
         <v>12</v>
       </c>
       <c r="C67" s="18" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D67" s="18" t="e">
         <f>Preg_Respuestas!D67</f>
@@ -33462,7 +33618,7 @@
         <v>12</v>
       </c>
       <c r="C68" s="18" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D68" s="18" t="e">
         <f>Preg_Respuestas!D68</f>
@@ -33478,7 +33634,7 @@
         <v>13</v>
       </c>
       <c r="C69" s="18" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D69" s="18" t="e">
         <f>Preg_Respuestas!D69</f>
@@ -33494,7 +33650,7 @@
         <v>13</v>
       </c>
       <c r="C70" s="18" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D70" s="18" t="e">
         <f>Preg_Respuestas!D70</f>
@@ -33510,7 +33666,7 @@
         <v>13</v>
       </c>
       <c r="C71" s="18" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D71" s="18" t="e">
         <f>Preg_Respuestas!D71</f>
@@ -34474,34 +34630,34 @@
   <sheetData>
     <row r="1" spans="1:10" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="11" t="s">
+        <v>35</v>
+      </c>
+      <c r="B1" s="19" t="s">
         <v>36</v>
       </c>
-      <c r="B1" s="19" t="s">
+      <c r="C1" s="20" t="s">
         <v>37</v>
       </c>
-      <c r="C1" s="20" t="s">
+      <c r="D1" s="20" t="s">
         <v>38</v>
       </c>
-      <c r="D1" s="20" t="s">
+      <c r="E1" s="21" t="s">
         <v>39</v>
       </c>
-      <c r="E1" s="21" t="s">
+      <c r="F1" s="22" t="s">
+        <v>24</v>
+      </c>
+      <c r="G1" s="23" t="s">
         <v>40</v>
       </c>
-      <c r="F1" s="22" t="s">
-        <v>25</v>
-      </c>
-      <c r="G1" s="23" t="s">
+      <c r="H1" s="24" t="s">
         <v>41</v>
       </c>
-      <c r="H1" s="24" t="s">
+      <c r="I1" s="24" t="s">
         <v>42</v>
       </c>
-      <c r="I1" s="24" t="s">
-        <v>43</v>
-      </c>
       <c r="J1" s="24" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="2" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -35569,19 +35725,19 @@
   <sheetData>
     <row r="1" spans="1:5" ht="36.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="17" t="s">
+        <v>43</v>
+      </c>
+      <c r="B1" s="17" t="s">
         <v>44</v>
       </c>
-      <c r="B1" s="17" t="s">
+      <c r="C1" s="17" t="s">
         <v>45</v>
       </c>
-      <c r="C1" s="17" t="s">
+      <c r="D1" s="17" t="s">
         <v>46</v>
       </c>
-      <c r="D1" s="17" t="s">
+      <c r="E1" s="17" t="s">
         <v>47</v>
-      </c>
-      <c r="E1" s="17" t="s">
-        <v>48</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -37912,22 +38068,22 @@
   <sheetData>
     <row r="1" spans="1:6" ht="26.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="19" t="s">
+        <v>48</v>
+      </c>
+      <c r="B1" s="20" t="s">
         <v>49</v>
       </c>
-      <c r="B1" s="20" t="s">
+      <c r="C1" s="20" t="s">
         <v>50</v>
       </c>
-      <c r="C1" s="20" t="s">
+      <c r="D1" s="21" t="s">
         <v>51</v>
       </c>
-      <c r="D1" s="21" t="s">
+      <c r="E1" s="22" t="s">
+        <v>24</v>
+      </c>
+      <c r="F1" s="22" t="s">
         <v>52</v>
-      </c>
-      <c r="E1" s="22" t="s">
-        <v>25</v>
-      </c>
-      <c r="F1" s="22" t="s">
-        <v>53</v>
       </c>
     </row>
     <row r="2" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -38983,16 +39139,16 @@
   <sheetData>
     <row r="1" spans="1:26" ht="27" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="17" t="s">
+        <v>44</v>
+      </c>
+      <c r="B1" s="17" t="s">
         <v>45</v>
       </c>
-      <c r="B1" s="17" t="s">
-        <v>46</v>
-      </c>
       <c r="C1" s="17" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D1" s="32" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="E1" s="33"/>
       <c r="F1" s="33"/>
@@ -41132,25 +41288,25 @@
   <sheetData>
     <row r="1" spans="1:9" ht="21.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="34" t="s">
+        <v>54</v>
+      </c>
+      <c r="B1" s="35" t="s">
         <v>55</v>
       </c>
-      <c r="B1" s="35" t="s">
+      <c r="C1" s="35" t="s">
         <v>56</v>
       </c>
-      <c r="C1" s="35" t="s">
+      <c r="D1" s="36" t="s">
         <v>57</v>
       </c>
-      <c r="D1" s="36" t="s">
+      <c r="E1" s="36" t="s">
+        <v>53</v>
+      </c>
+      <c r="F1" s="36" t="s">
         <v>58</v>
       </c>
-      <c r="E1" s="36" t="s">
-        <v>54</v>
-      </c>
-      <c r="F1" s="36" t="s">
+      <c r="G1" s="37" t="s">
         <v>59</v>
-      </c>
-      <c r="G1" s="37" t="s">
-        <v>60</v>
       </c>
       <c r="I1" s="38"/>
     </row>
@@ -41176,7 +41332,7 @@
         <v>#REF!</v>
       </c>
       <c r="F2" s="42" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="G2" s="44" t="e">
         <f t="shared" ref="G2:G46" si="2">IF(AND(#REF!="C",NOT(ISBLANK(#REF!))),#REF!)</f>
@@ -41206,7 +41362,7 @@
         <v>#REF!</v>
       </c>
       <c r="F3" s="42" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="G3" s="44" t="e">
         <f t="shared" si="2"/>
@@ -41236,7 +41392,7 @@
         <v>#REF!</v>
       </c>
       <c r="F4" s="42" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="G4" s="44" t="e">
         <f t="shared" si="2"/>
@@ -41266,7 +41422,7 @@
         <v>#REF!</v>
       </c>
       <c r="F5" s="42" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="G5" s="44" t="e">
         <f t="shared" si="2"/>
@@ -41296,7 +41452,7 @@
         <v>#REF!</v>
       </c>
       <c r="F6" s="42" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="G6" s="44" t="e">
         <f t="shared" si="2"/>
@@ -41326,7 +41482,7 @@
         <v>#REF!</v>
       </c>
       <c r="F7" s="42" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="G7" s="44" t="e">
         <f t="shared" si="2"/>
@@ -41356,7 +41512,7 @@
         <v>#REF!</v>
       </c>
       <c r="F8" s="42" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="G8" s="44" t="e">
         <f t="shared" si="2"/>
@@ -41386,7 +41542,7 @@
         <v>#REF!</v>
       </c>
       <c r="F9" s="42" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="G9" s="44" t="e">
         <f t="shared" si="2"/>
@@ -41416,7 +41572,7 @@
         <v>#REF!</v>
       </c>
       <c r="F10" s="42" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="G10" s="44" t="e">
         <f t="shared" si="2"/>
@@ -41446,7 +41602,7 @@
         <v>#REF!</v>
       </c>
       <c r="F11" s="42" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="G11" s="44" t="e">
         <f t="shared" si="2"/>
@@ -41476,7 +41632,7 @@
         <v>#REF!</v>
       </c>
       <c r="F12" s="42" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="G12" s="44" t="e">
         <f t="shared" si="2"/>
@@ -41506,7 +41662,7 @@
         <v>#REF!</v>
       </c>
       <c r="F13" s="42" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="G13" s="44" t="e">
         <f t="shared" si="2"/>
@@ -41536,7 +41692,7 @@
         <v>#REF!</v>
       </c>
       <c r="F14" s="42" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="G14" s="44" t="e">
         <f t="shared" si="2"/>
@@ -41566,7 +41722,7 @@
         <v>#REF!</v>
       </c>
       <c r="F15" s="42" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="G15" s="44" t="e">
         <f t="shared" si="2"/>
@@ -41596,7 +41752,7 @@
         <v>#REF!</v>
       </c>
       <c r="F16" s="42" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="G16" s="44" t="e">
         <f t="shared" si="2"/>
@@ -41626,7 +41782,7 @@
         <v>#REF!</v>
       </c>
       <c r="F17" s="42" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="G17" s="44" t="e">
         <f t="shared" si="2"/>
@@ -41656,7 +41812,7 @@
         <v>#REF!</v>
       </c>
       <c r="F18" s="42" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="G18" s="44" t="e">
         <f t="shared" si="2"/>
@@ -41686,7 +41842,7 @@
         <v>#REF!</v>
       </c>
       <c r="F19" s="42" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="G19" s="44" t="e">
         <f t="shared" si="2"/>
@@ -41716,7 +41872,7 @@
         <v>#REF!</v>
       </c>
       <c r="F20" s="42" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="G20" s="44" t="e">
         <f t="shared" si="2"/>
@@ -41746,7 +41902,7 @@
         <v>#REF!</v>
       </c>
       <c r="F21" s="42" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="G21" s="44" t="e">
         <f t="shared" si="2"/>
@@ -41776,7 +41932,7 @@
         <v>#REF!</v>
       </c>
       <c r="F22" s="42" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="G22" s="44" t="e">
         <f t="shared" si="2"/>
@@ -41806,7 +41962,7 @@
         <v>#REF!</v>
       </c>
       <c r="F23" s="42" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="G23" s="44" t="e">
         <f t="shared" si="2"/>
@@ -41836,7 +41992,7 @@
         <v>#REF!</v>
       </c>
       <c r="F24" s="42" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="G24" s="44" t="e">
         <f t="shared" si="2"/>
@@ -41866,7 +42022,7 @@
         <v>#REF!</v>
       </c>
       <c r="F25" s="42" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="G25" s="44" t="e">
         <f t="shared" si="2"/>
@@ -41896,7 +42052,7 @@
         <v>#REF!</v>
       </c>
       <c r="F26" s="42" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="G26" s="44" t="e">
         <f t="shared" si="2"/>
@@ -41926,7 +42082,7 @@
         <v>#REF!</v>
       </c>
       <c r="F27" s="42" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="G27" s="44" t="e">
         <f t="shared" si="2"/>
@@ -41956,7 +42112,7 @@
         <v>#REF!</v>
       </c>
       <c r="F28" s="42" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="G28" s="44" t="e">
         <f t="shared" si="2"/>
@@ -41986,7 +42142,7 @@
         <v>#REF!</v>
       </c>
       <c r="F29" s="42" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="G29" s="44" t="e">
         <f t="shared" si="2"/>
@@ -42016,7 +42172,7 @@
         <v>#REF!</v>
       </c>
       <c r="F30" s="42" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="G30" s="44" t="e">
         <f t="shared" si="2"/>
@@ -42046,7 +42202,7 @@
         <v>#REF!</v>
       </c>
       <c r="F31" s="42" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="G31" s="44" t="e">
         <f t="shared" si="2"/>
@@ -42076,7 +42232,7 @@
         <v>#REF!</v>
       </c>
       <c r="F32" s="42" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="G32" s="44" t="e">
         <f t="shared" si="2"/>
@@ -42106,7 +42262,7 @@
         <v>#REF!</v>
       </c>
       <c r="F33" s="42" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="G33" s="44" t="e">
         <f t="shared" si="2"/>
@@ -42136,7 +42292,7 @@
         <v>#REF!</v>
       </c>
       <c r="F34" s="42" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="G34" s="44" t="e">
         <f t="shared" si="2"/>
@@ -42166,7 +42322,7 @@
         <v>#REF!</v>
       </c>
       <c r="F35" s="42" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="G35" s="44" t="e">
         <f t="shared" si="2"/>
@@ -42196,7 +42352,7 @@
         <v>#REF!</v>
       </c>
       <c r="F36" s="42" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="G36" s="44" t="e">
         <f t="shared" si="2"/>
@@ -42226,7 +42382,7 @@
         <v>#REF!</v>
       </c>
       <c r="F37" s="42" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="G37" s="44" t="e">
         <f t="shared" si="2"/>
@@ -42256,7 +42412,7 @@
         <v>#REF!</v>
       </c>
       <c r="F38" s="42" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="G38" s="44" t="e">
         <f t="shared" si="2"/>
@@ -42286,7 +42442,7 @@
         <v>#REF!</v>
       </c>
       <c r="F39" s="42" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="G39" s="44" t="e">
         <f t="shared" si="2"/>
@@ -42316,7 +42472,7 @@
         <v>#REF!</v>
       </c>
       <c r="F40" s="42" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="G40" s="44" t="e">
         <f t="shared" si="2"/>
@@ -42346,7 +42502,7 @@
         <v>#REF!</v>
       </c>
       <c r="F41" s="42" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="G41" s="44" t="e">
         <f t="shared" si="2"/>
@@ -42376,7 +42532,7 @@
         <v>#REF!</v>
       </c>
       <c r="F42" s="42" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="G42" s="44" t="e">
         <f t="shared" si="2"/>
@@ -42406,7 +42562,7 @@
         <v>#REF!</v>
       </c>
       <c r="F43" s="42" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="G43" s="44" t="e">
         <f t="shared" si="2"/>
@@ -42436,7 +42592,7 @@
         <v>#REF!</v>
       </c>
       <c r="F44" s="42" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="G44" s="44" t="e">
         <f t="shared" si="2"/>
@@ -42466,7 +42622,7 @@
         <v>#REF!</v>
       </c>
       <c r="F45" s="42" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="G45" s="44" t="e">
         <f t="shared" si="2"/>
@@ -42496,7 +42652,7 @@
         <v>#REF!</v>
       </c>
       <c r="F46" s="42" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="G46" s="44" t="e">
         <f t="shared" si="2"/>
@@ -46490,9 +46646,15 @@
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D80E8597-937D-4506-AE34-60733D3C3BD7}">
   <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="f9f3b390-cc4e-48c6-b220-f74dc9f0acc5"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="f9f3b390-cc4e-48c6-b220-f74dc9f0acc5"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>